<commit_message>
Password is changed in Excel
</commit_message>
<xml_diff>
--- a/src/test/resource/TestData/testDataSheet.xlsx
+++ b/src/test/resource/TestData/testDataSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -51,7 +51,7 @@
     <t>test@gmail.com</t>
   </si>
   <si>
-    <t>Test123</t>
+    <t>Test1234</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Steps in "SearchPageTest" to retrieve Skills and Location from the Excel sheet. Added a method named "getExcelTest" in the BasePageObject.java for the same.
</commit_message>
<xml_diff>
--- a/src/test/resource/TestData/testDataSheet.xlsx
+++ b/src/test/resource/TestData/testDataSheet.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="11325" windowHeight="3525"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:K10"/>
 </workbook>
 </file>
 
@@ -57,8 +58,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,7 +199,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -233,7 +233,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,20 +408,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -460,20 +459,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -504,12 +503,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Steps in "RegisterPageTest" to get data from Excel sheet.And deleted the same entries from the "NKConstants" util.
</commit_message>
<xml_diff>
--- a/src/test/resource/TestData/testDataSheet.xlsx
+++ b/src/test/resource/TestData/testDataSheet.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="11325" windowHeight="3525"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="11325" windowHeight="3525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:K10"/>
+  <oleSize ref="A1:F10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>TC_ID</t>
   </si>
@@ -53,6 +53,102 @@
   </si>
   <si>
     <t>Test1234</t>
+  </si>
+  <si>
+    <t>password_invalid</t>
+  </si>
+  <si>
+    <t>password_valid</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>mobileNumber_valid</t>
+  </si>
+  <si>
+    <t>mobileNumber_invalid</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>basicEducation</t>
+  </si>
+  <si>
+    <t>filePath_invalid</t>
+  </si>
+  <si>
+    <t>filePath_valid</t>
+  </si>
+  <si>
+    <t>resumeText</t>
+  </si>
+  <si>
+    <t>specialization</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>yearOfCompletion</t>
+  </si>
+  <si>
+    <t>currentIndustry</t>
+  </si>
+  <si>
+    <t>functionalArea</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>jobAlertName</t>
+  </si>
+  <si>
+    <t>aks</t>
+  </si>
+  <si>
+    <t>godisking</t>
+  </si>
+  <si>
+    <t>Senior Software Engineer</t>
+  </si>
+  <si>
+    <t>B.Tech/B.E.</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Admin\\Desktop\\resume.txt</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Admin\\Desktop\\resume.docx</t>
+  </si>
+  <si>
+    <t>My Resume</t>
+  </si>
+  <si>
+    <t>Computers</t>
+  </si>
+  <si>
+    <t>Anna University</t>
+  </si>
+  <si>
+    <t>IT-Software/Software Services</t>
+  </si>
+  <si>
+    <t>IT Software - Application Programming / Maintenance</t>
+  </si>
+  <si>
+    <t>Testing Engnr</t>
+  </si>
+  <si>
+    <t>MyAlert</t>
+  </si>
+  <si>
+    <t>mukeshkumar</t>
   </si>
 </sst>
 </file>
@@ -411,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -451,6 +547,9 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -462,9 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -504,12 +601,145 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2">
+        <v>12345</v>
+      </c>
+      <c r="F2">
+        <v>9900224430</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2">
+        <v>2005</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>